<commit_message>
- Implemented motor insert and delete functionality. - Added program icon
</commit_message>
<xml_diff>
--- a/V1000_Drive_Programmer/data/MOTOR_DATA.xlsx
+++ b/V1000_Drive_Programmer/data/MOTOR_DATA.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4725" yWindow="0" windowWidth="28800" windowHeight="12915"/>
+    <workbookView xWindow="16065" yWindow="0" windowWidth="28800" windowHeight="12915"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -393,11 +393,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R34"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
+  <dimension ref="A1:R35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0" rightToLeft="false">
+      <selection activeCell="A35" sqref="A35:XFD35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -406,7 +406,7 @@
     <col min="3" max="32" width="12.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row spans="1:18" x14ac:dyDescent="0.2" outlineLevel="0" r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -462,7 +462,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row spans="1:18" x14ac:dyDescent="0.2" outlineLevel="0" r="2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -509,7 +509,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row spans="1:18" x14ac:dyDescent="0.2" outlineLevel="0" r="3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -517,34 +517,34 @@
         <v>55090</v>
       </c>
       <c r="C3">
-        <v>9.1999999999999993</v>
+        <v>9.2</v>
       </c>
       <c r="E3">
-        <v>9.1999999999999993</v>
+        <v>9.2</v>
       </c>
       <c r="F3">
         <v>8.1</v>
       </c>
       <c r="H3">
-        <v>8.0500000000000007</v>
+        <v>8.05</v>
       </c>
       <c r="J3">
         <v>8</v>
       </c>
       <c r="M3">
-        <v>4.5999999999999996</v>
+        <v>4.6</v>
       </c>
       <c r="O3">
-        <v>4.5999999999999996</v>
+        <v>4.6</v>
       </c>
       <c r="P3">
-        <v>4.5999999999999996</v>
+        <v>4.6</v>
       </c>
       <c r="Q3">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+    <row spans="1:18" x14ac:dyDescent="0.2" outlineLevel="0" r="4">
       <c r="A4">
         <v>2</v>
       </c>
@@ -561,10 +561,10 @@
         <v>10.6</v>
       </c>
       <c r="F4">
-        <v>9.3000000000000007</v>
+        <v>9.3</v>
       </c>
       <c r="H4">
-        <v>8.8000000000000007</v>
+        <v>8.8</v>
       </c>
       <c r="J4">
         <v>8.4</v>
@@ -573,7 +573,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    <row spans="1:18" x14ac:dyDescent="0.2" outlineLevel="0" r="5">
       <c r="A5">
         <v>3</v>
       </c>
@@ -596,7 +596,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row spans="1:18" x14ac:dyDescent="0.2" outlineLevel="0" r="6">
       <c r="A6">
         <v>4</v>
       </c>
@@ -634,7 +634,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+    <row spans="1:18" x14ac:dyDescent="0.2" outlineLevel="0" r="7">
       <c r="A7">
         <v>5</v>
       </c>
@@ -666,7 +666,7 @@
         <v>6.8</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    <row spans="1:18" x14ac:dyDescent="0.2" outlineLevel="0" r="8">
       <c r="A8">
         <v>6</v>
       </c>
@@ -686,7 +686,7 @@
         <v>14.5</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+    <row spans="1:18" x14ac:dyDescent="0.2" outlineLevel="0" r="9">
       <c r="A9">
         <v>7</v>
       </c>
@@ -706,7 +706,7 @@
         <v>15.2</v>
       </c>
       <c r="M9">
-        <v>8.3000000000000007</v>
+        <v>8.3</v>
       </c>
       <c r="N9">
         <v>7.5</v>
@@ -715,10 +715,10 @@
         <v>8.59</v>
       </c>
       <c r="P9">
-        <v>8.8000000000000007</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+        <v>8.8</v>
+      </c>
+    </row>
+    <row spans="1:18" x14ac:dyDescent="0.2" outlineLevel="0" r="10">
       <c r="A10">
         <v>8</v>
       </c>
@@ -738,7 +738,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    <row spans="1:18" x14ac:dyDescent="0.2" outlineLevel="0" r="11">
       <c r="A11">
         <v>9</v>
       </c>
@@ -770,7 +770,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+    <row spans="1:18" x14ac:dyDescent="0.2" outlineLevel="0" r="12">
       <c r="A12">
         <v>10</v>
       </c>
@@ -802,7 +802,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    <row spans="1:18" x14ac:dyDescent="0.2" outlineLevel="0" r="13">
       <c r="A13">
         <v>11</v>
       </c>
@@ -834,7 +834,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+    <row spans="1:18" x14ac:dyDescent="0.2" outlineLevel="0" r="14">
       <c r="A14">
         <v>12</v>
       </c>
@@ -866,7 +866,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+    <row spans="1:18" x14ac:dyDescent="0.2" outlineLevel="0" r="15">
       <c r="A15">
         <v>13</v>
       </c>
@@ -895,7 +895,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+    <row spans="1:18" x14ac:dyDescent="0.2" outlineLevel="0" r="16">
       <c r="A16">
         <v>14</v>
       </c>
@@ -906,19 +906,19 @@
         <v>12</v>
       </c>
       <c r="D16">
-        <v>9.6999999999999993</v>
+        <v>9.7</v>
       </c>
       <c r="E16">
         <v>11.6</v>
       </c>
       <c r="F16">
-        <v>9.3000000000000007</v>
+        <v>9.3</v>
       </c>
       <c r="G16">
         <v>11</v>
       </c>
       <c r="H16">
-        <v>8.6999999999999993</v>
+        <v>8.7</v>
       </c>
       <c r="M16">
         <v>6.4</v>
@@ -927,7 +927,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+    <row spans="1:17" x14ac:dyDescent="0.2" outlineLevel="0" r="17">
       <c r="A17">
         <v>15</v>
       </c>
@@ -956,7 +956,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+    <row spans="1:17" x14ac:dyDescent="0.2" outlineLevel="0" r="18">
       <c r="A18">
         <v>16</v>
       </c>
@@ -967,19 +967,19 @@
         <v>12</v>
       </c>
       <c r="D18">
-        <v>9.6999999999999993</v>
+        <v>9.7</v>
       </c>
       <c r="E18">
         <v>11.6</v>
       </c>
       <c r="F18">
-        <v>9.3000000000000007</v>
+        <v>9.3</v>
       </c>
       <c r="G18">
         <v>11</v>
       </c>
       <c r="H18">
-        <v>8.6999999999999993</v>
+        <v>8.7</v>
       </c>
       <c r="M18">
         <v>6.4</v>
@@ -988,7 +988,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+    <row spans="1:17" x14ac:dyDescent="0.2" outlineLevel="0" r="19">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1014,7 +1014,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+    <row spans="1:17" x14ac:dyDescent="0.2" outlineLevel="0" r="20">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1025,7 +1025,7 @@
         <v>2.8</v>
       </c>
       <c r="H20">
-        <v>2.2999999999999998</v>
+        <v>2.3</v>
       </c>
       <c r="I20">
         <v>2.85</v>
@@ -1052,7 +1052,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+    <row spans="1:17" x14ac:dyDescent="0.2" outlineLevel="0" r="21">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1072,7 +1072,7 @@
         <v>5.4</v>
       </c>
       <c r="I21">
-        <v>5.0999999999999996</v>
+        <v>5.1</v>
       </c>
       <c r="J21">
         <v>5.2</v>
@@ -1093,7 +1093,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+    <row spans="1:17" x14ac:dyDescent="0.2" outlineLevel="0" r="22">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1107,7 +1107,7 @@
         <v>16.8</v>
       </c>
       <c r="E22">
-        <v>19.100000000000001</v>
+        <v>19.1</v>
       </c>
       <c r="F22">
         <v>16.21</v>
@@ -1122,7 +1122,7 @@
         <v>7.3</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+    <row spans="1:17" x14ac:dyDescent="0.2" outlineLevel="0" r="23">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1145,7 +1145,7 @@
         <v>8.5</v>
       </c>
       <c r="N23">
-        <v>8.1999999999999993</v>
+        <v>8.2</v>
       </c>
       <c r="O23">
         <v>8.56</v>
@@ -1154,7 +1154,7 @@
         <v>8.6</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+    <row spans="1:17" x14ac:dyDescent="0.2" outlineLevel="0" r="24">
       <c r="A24">
         <v>22</v>
       </c>
@@ -1162,7 +1162,7 @@
         <v>51690</v>
       </c>
       <c r="G24">
-        <v>8.8000000000000007</v>
+        <v>8.8</v>
       </c>
       <c r="H24">
         <v>8.1</v>
@@ -1174,7 +1174,7 @@
         <v>9.5</v>
       </c>
       <c r="M24">
-        <v>5.0999999999999996</v>
+        <v>5.1</v>
       </c>
       <c r="N24">
         <v>4.7</v>
@@ -1186,7 +1186,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+    <row spans="1:17" x14ac:dyDescent="0.2" outlineLevel="0" r="25">
       <c r="A25">
         <v>23</v>
       </c>
@@ -1194,19 +1194,19 @@
         <v>51691</v>
       </c>
       <c r="C25">
-        <v>9.1999999999999993</v>
+        <v>9.2</v>
       </c>
       <c r="D25">
         <v>8.6</v>
       </c>
       <c r="E25">
-        <v>9.1999999999999993</v>
+        <v>9.2</v>
       </c>
       <c r="F25">
         <v>8.44</v>
       </c>
       <c r="H25">
-        <v>8.1999999999999993</v>
+        <v>8.2</v>
       </c>
       <c r="J25">
         <v>8</v>
@@ -1215,7 +1215,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+    <row spans="1:17" x14ac:dyDescent="0.2" outlineLevel="0" r="26">
       <c r="A26">
         <v>24</v>
       </c>
@@ -1244,7 +1244,7 @@
         <v>13.8</v>
       </c>
       <c r="M26">
-        <v>8.3000000000000007</v>
+        <v>8.3</v>
       </c>
       <c r="O26">
         <v>7.9</v>
@@ -1256,7 +1256,7 @@
         <v>6.9</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+    <row spans="1:17" x14ac:dyDescent="0.2" outlineLevel="0" r="27">
       <c r="A27">
         <v>25</v>
       </c>
@@ -1270,7 +1270,7 @@
         <v>14.2</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+    <row spans="1:17" x14ac:dyDescent="0.2" outlineLevel="0" r="28">
       <c r="A28">
         <v>26</v>
       </c>
@@ -1281,7 +1281,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+    <row spans="1:17" x14ac:dyDescent="0.2" outlineLevel="0" r="29">
       <c r="A29">
         <v>27</v>
       </c>
@@ -1292,7 +1292,7 @@
         <v>4.2</v>
       </c>
       <c r="E29">
-        <v>4.0599999999999996</v>
+        <v>4.06</v>
       </c>
       <c r="G29">
         <v>3.85</v>
@@ -1304,7 +1304,7 @@
         <v>3.5</v>
       </c>
       <c r="M29">
-        <v>2.2000000000000002</v>
+        <v>2.2</v>
       </c>
       <c r="N29">
         <v>1.9</v>
@@ -1319,7 +1319,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+    <row spans="1:17" x14ac:dyDescent="0.2" outlineLevel="0" r="30">
       <c r="A30">
         <v>28</v>
       </c>
@@ -1327,7 +1327,7 @@
         <v>58225</v>
       </c>
       <c r="D30">
-        <v>4.9000000000000004</v>
+        <v>4.9</v>
       </c>
       <c r="F30">
         <v>4.74</v>
@@ -1342,7 +1342,7 @@
         <v>4.12</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+    <row spans="1:17" x14ac:dyDescent="0.2" outlineLevel="0" r="31">
       <c r="A31">
         <v>29</v>
       </c>
@@ -1350,13 +1350,13 @@
         <v>58393</v>
       </c>
       <c r="C31">
-        <v>9.3000000000000007</v>
+        <v>9.3</v>
       </c>
       <c r="E31">
         <v>9</v>
       </c>
       <c r="G31">
-        <v>8.5500000000000007</v>
+        <v>8.55</v>
       </c>
       <c r="I31">
         <v>8.18</v>
@@ -1365,10 +1365,10 @@
         <v>7.8</v>
       </c>
       <c r="M31">
-        <v>4.9000000000000004</v>
+        <v>4.9</v>
       </c>
       <c r="N31">
-        <v>4.9000000000000004</v>
+        <v>4.9</v>
       </c>
       <c r="O31">
         <v>4.67</v>
@@ -1380,7 +1380,7 @@
         <v>4.05</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+    <row spans="1:17" x14ac:dyDescent="0.2" outlineLevel="0" r="32">
       <c r="A32">
         <v>30</v>
       </c>
@@ -1388,13 +1388,13 @@
         <v>58394</v>
       </c>
       <c r="D32">
-        <v>9.3000000000000007</v>
+        <v>9.3</v>
       </c>
       <c r="F32">
         <v>9</v>
       </c>
       <c r="H32">
-        <v>8.5500000000000007</v>
+        <v>8.55</v>
       </c>
       <c r="J32">
         <v>8.18</v>
@@ -1406,7 +1406,7 @@
         <v>4.05</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
+    <row spans="1:17" x14ac:dyDescent="0.2" outlineLevel="0" r="33">
       <c r="A33">
         <v>31</v>
       </c>
@@ -1438,7 +1438,7 @@
         <v>2.9</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
+    <row spans="1:17" x14ac:dyDescent="0.2" outlineLevel="0" r="34">
       <c r="A34">
         <v>32</v>
       </c>
@@ -1468,6 +1468,17 @@
       </c>
       <c r="Q34">
         <v>2.9</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="35">
+      <c r="A35" s="0">
+        <v>33</v>
+      </c>
+      <c r="B35" s="0">
+        <v>16554</v>
+      </c>
+      <c r="H35" s="0">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>